<commit_message>
Add awards mechanism (no display yet)
</commit_message>
<xml_diff>
--- a/statistics-for-all-workers.xlsx
+++ b/statistics-for-all-workers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sebastien\Documents\Concordia\CART415\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sebastien\Documents\Concordia\CART415\roller-clicker-tycoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14498BB9-8BBD-4949-B4EC-4B67D0536DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8477E323-1AC4-476E-AE0A-8E68D659EC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C88C3EED-B264-4854-BD81-362B22C2E55B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>Rides</t>
   </si>
@@ -121,6 +121,93 @@
   </si>
   <si>
     <t>Rebate</t>
+  </si>
+  <si>
+    <t>Awards</t>
+  </si>
+  <si>
+    <t>Toute le Kébec!</t>
+  </si>
+  <si>
+    <t>Mr. Worldwide!</t>
+  </si>
+  <si>
+    <t>We all start somewhere!</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>You got your first guest!</t>
+  </si>
+  <si>
+    <t>The entire Québec population is in your park!</t>
+  </si>
+  <si>
+    <t>The entire US population is in your park!</t>
+  </si>
+  <si>
+    <t>The entire Canada population is in your park!</t>
+  </si>
+  <si>
+    <t>Freedom isn't Free!</t>
+  </si>
+  <si>
+    <t>Le Québec n'est pas un pays!</t>
+  </si>
+  <si>
+    <t>Sa poud</t>
+  </si>
+  <si>
+    <t>A+ management</t>
+  </si>
+  <si>
+    <t>More Flags, More Fun!</t>
+  </si>
+  <si>
+    <t>Your park has as many guests as Six Flags Magic Mountain received in 2019!</t>
+  </si>
+  <si>
+    <t>1 hour wait</t>
+  </si>
+  <si>
+    <t>The entire Sorel population is in your park!</t>
+  </si>
+  <si>
+    <t>Wooo, it's starting to get crowded in here.</t>
+  </si>
+  <si>
+    <t>Golden play button!</t>
+  </si>
+  <si>
+    <t>The entire world population is in your park! Nice job.</t>
+  </si>
+  <si>
+    <t>Chinatown</t>
+  </si>
+  <si>
+    <t>The entire China population is in your park!</t>
+  </si>
+  <si>
+    <t>A tenth of the way there!</t>
+  </si>
+  <si>
+    <t>You got 100000 visitors in your park!</t>
+  </si>
+  <si>
+    <t>You got 100 guests in your park!</t>
+  </si>
+  <si>
+    <t>You got 1000 guests in your park! Your coaster's lines shouldn't be too long.</t>
+  </si>
+  <si>
+    <t>Philly Cheese Steak</t>
+  </si>
+  <si>
+    <t>The entire Pittsburgh population is in your park!</t>
   </si>
 </sst>
 </file>
@@ -156,8 +243,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -472,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C45A61AC-E79F-4868-B7B6-CF691AF83DEE}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+    <sheetView tabSelected="1" topLeftCell="E19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="N35" sqref="N35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,12 +573,12 @@
     <col min="3" max="4" width="13" customWidth="1"/>
     <col min="6" max="6" width="26.85546875" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" customWidth="1"/>
+    <col min="14" max="14" width="40.5703125" customWidth="1"/>
+    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
@@ -775,7 +863,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>21</v>
       </c>
@@ -792,7 +880,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -815,7 +903,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>23</v>
       </c>
@@ -835,7 +923,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>24</v>
       </c>
@@ -855,7 +943,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>25</v>
       </c>
@@ -875,7 +963,165 @@
         <v>5</v>
       </c>
     </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>29</v>
+      </c>
+      <c r="M24" t="s">
+        <v>33</v>
+      </c>
+      <c r="N24" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>32</v>
+      </c>
+      <c r="N25" t="s">
+        <v>35</v>
+      </c>
+      <c r="O25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>42</v>
+      </c>
+      <c r="N26" t="s">
+        <v>54</v>
+      </c>
+      <c r="O26" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>45</v>
+      </c>
+      <c r="N27" t="s">
+        <v>55</v>
+      </c>
+      <c r="O27" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>41</v>
+      </c>
+      <c r="N28" t="s">
+        <v>46</v>
+      </c>
+      <c r="O28" s="1">
+        <v>34755</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>52</v>
+      </c>
+      <c r="N29" t="s">
+        <v>53</v>
+      </c>
+      <c r="O29" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M30" t="s">
+        <v>56</v>
+      </c>
+      <c r="N30" t="s">
+        <v>57</v>
+      </c>
+      <c r="O30" s="1">
+        <v>300000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M31" t="s">
+        <v>48</v>
+      </c>
+      <c r="N31" t="s">
+        <v>47</v>
+      </c>
+      <c r="O31" s="1">
+        <v>1000000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>30</v>
+      </c>
+      <c r="N32" t="s">
+        <v>36</v>
+      </c>
+      <c r="O32" s="1">
+        <v>8400000</v>
+      </c>
+    </row>
+    <row r="33" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M33" t="s">
+        <v>43</v>
+      </c>
+      <c r="N33" t="s">
+        <v>44</v>
+      </c>
+      <c r="O33" s="1">
+        <v>26700000</v>
+      </c>
+    </row>
+    <row r="34" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>40</v>
+      </c>
+      <c r="N34" t="s">
+        <v>38</v>
+      </c>
+      <c r="O34" s="1">
+        <v>38000000</v>
+      </c>
+    </row>
+    <row r="35" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M35" t="s">
+        <v>39</v>
+      </c>
+      <c r="N35" t="s">
+        <v>37</v>
+      </c>
+      <c r="O35" s="1">
+        <v>330000000</v>
+      </c>
+    </row>
+    <row r="36" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>50</v>
+      </c>
+      <c r="N36" t="s">
+        <v>51</v>
+      </c>
+      <c r="O36" s="1">
+        <v>1402000000</v>
+      </c>
+    </row>
+    <row r="37" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>31</v>
+      </c>
+      <c r="N37" t="s">
+        <v>49</v>
+      </c>
+      <c r="O37" s="1">
+        <v>7753000000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>